<commit_message>
many failed attempts to complete the pest data merger, some preliminary analysis- scatter matrix, a few boxplots, etc.
</commit_message>
<xml_diff>
--- a/results/nightly_distribution_passes_graph.xlsx
+++ b/results/nightly_distribution_passes_graph.xlsx
@@ -1758,11 +1758,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2130031064"/>
-        <c:axId val="2126612040"/>
+        <c:axId val="-2092529080"/>
+        <c:axId val="-2092503848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130031064"/>
+        <c:axId val="-2092529080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1791,7 +1791,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126612040"/>
+        <c:crossAx val="-2092503848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1799,13 +1799,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126612040"/>
+        <c:axId val="-2092503848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1829,7 +1828,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130031064"/>
+        <c:crossAx val="-2092529080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1855,16 +1854,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2210,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>